<commit_message>
sensactUP2, sensactHsNano sensactHsLED sensactOutdoor as ordered at JLCPCB
</commit_message>
<xml_diff>
--- a/pcb/sensactOutdoor/A6211-Design-Tool.xlsx
+++ b/pcb/sensactOutdoor/A6211-Design-Tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\sensact\pcb\sensactOutdoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77D7994-D64A-4690-B5BA-EFE23C1043CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9AF985-58C4-47A7-8584-8EE7B140DF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28125" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component Calculator" sheetId="1" r:id="rId1"/>
@@ -2879,8 +2879,8 @@
   </sheetPr>
   <dimension ref="A1:GU86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3031,7 +3031,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="87">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>20</v>
@@ -3060,7 +3060,7 @@
       <c r="B16" s="10"/>
       <c r="C16" s="13">
         <f>C14*C15/100</f>
-        <v>0.21</v>
+        <v>0.09</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>24</v>
@@ -3282,7 +3282,7 @@
       <c r="B24" s="10"/>
       <c r="C24" s="29">
         <f>C19/C14</f>
-        <v>0.28571428571428575</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>46</v>
@@ -3513,7 +3513,7 @@
         <v>49</v>
       </c>
       <c r="C25" s="88">
-        <v>0.3</v>
+        <v>0.68</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>46</v>
@@ -3743,7 +3743,7 @@
       </c>
       <c r="C26" s="35">
         <f>C19/C25</f>
-        <v>0.66666666666666674</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>20</v>
@@ -5740,7 +5740,7 @@
       <c r="B35" s="16"/>
       <c r="C35" s="40">
         <f>(C10-C13)*C31/C16</f>
-        <v>38.806759126984126</v>
+        <v>90.549104629629625</v>
       </c>
       <c r="D35" t="s">
         <v>68</v>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="C38" s="53">
         <f>(C26+C37/2) * 1.2</f>
-        <v>0.9040351414893617</v>
+        <v>0.45697631795994997</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>20</v>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="C39" s="57">
         <f>C37*C25</f>
-        <v>5.2017570744680851E-2</v>
+        <v>0.11790649368794327</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>79</v>
@@ -7500,11 +7500,11 @@
     <row r="43" spans="1:203" x14ac:dyDescent="0.2">
       <c r="A43" s="72" t="str">
         <f xml:space="preserve"> "Average LED current with Rs= " &amp; TEXT(C25,"###") &amp; "mOhm"</f>
-        <v>Average LED current with Rs= mOhm</v>
+        <v>Average LED current with Rs= 1mOhm</v>
       </c>
       <c r="C43" s="60">
         <f>C26</f>
-        <v>0.66666666666666674</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>20</v>
@@ -7927,7 +7927,7 @@
       </c>
       <c r="C45" s="63">
         <f>C44*100/C43</f>
-        <v>26.008785372340427</v>
+        <v>58.953246843971634</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="C55" s="79">
         <f>C26</f>
-        <v>0.66666666666666674</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
@@ -8076,7 +8076,7 @@
       </c>
       <c r="C56" s="81">
         <f>C55*C55*C51*(1+C52) * C54</f>
-        <v>0.178509373571102</v>
+        <v>3.47444714995657E-2</v>
       </c>
       <c r="D56" t="s">
         <v>104</v>
@@ -8152,7 +8152,7 @@
       </c>
       <c r="C61" s="81">
         <f>C49*C55*(C59+C60)/2000 *C58</f>
-        <v>0.33204205866076369</v>
+        <v>0.14648914352680753</v>
       </c>
       <c r="D61" t="s">
         <v>104</v>
@@ -8175,7 +8175,7 @@
       </c>
       <c r="C63" s="81">
         <f>C56+C61</f>
-        <v>0.51055143223186572</v>
+        <v>0.18123361502637322</v>
       </c>
       <c r="D63" t="s">
         <v>104</v>
@@ -8203,7 +8203,7 @@
       </c>
       <c r="C64" s="83">
         <f>C63*C50</f>
-        <v>17.869300128115299</v>
+        <v>6.343176525923063</v>
       </c>
       <c r="D64" s="66" t="s">
         <v>119</v>
@@ -8268,7 +8268,7 @@
       </c>
       <c r="C66" s="82">
         <f>C65+C64</f>
-        <v>102.8693001281153</v>
+        <v>91.34317652592307</v>
       </c>
       <c r="D66" s="66" t="s">
         <v>119</v>

</xml_diff>